<commit_message>
Refactoring and cases addition
</commit_message>
<xml_diff>
--- a/src/test/java/MarketData_OPT_L1/Data/MarketData_OPT_L1.xlsx
+++ b/src/test/java/MarketData_OPT_L1/Data/MarketData_OPT_L1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmal.syed.LOGICIELSERVICE\eclipse-workspace\OMS_API\src\test\java\MarketData_OPT_L1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APIAutomation\Automation_OMSAPI\src\test\java\MarketData_OPT_L1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395E2FB5-CCC3-4E10-AC20-1E95426E4EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E68443A-E187-45CF-8912-7A57B24D72F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="584" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Topic" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="115">
   <si>
     <t>Topic_Base_Path</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Subscribe_TestCases</t>
   </si>
   <si>
-    <t>Verify_Opt_Subscribe_MarketData_TC0001</t>
-  </si>
-  <si>
     <t>Verify_Opt_UnSubscribe_MarketData_TC0001</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>Subscribe_Bulk_TestCases</t>
   </si>
   <si>
-    <t>Verify_Opt_Subscribe_Bulk_MarketData_TC0001</t>
-  </si>
-  <si>
     <t>UnSubscribe_Bulk_TestCases</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>UnSubscribe_Bulk_Symbol_TestCases</t>
   </si>
   <si>
-    <t>Verify_Opt_Topic_TC0001</t>
-  </si>
-  <si>
     <t>[CustomStatus, CloseCondition, LastSize, PreviousNetChange, CloseDate, PreviousClose, ShortSalePriceRestricted, PreviousBid, QuoteDate, PreviousCumulativePrice, PreviousOpen, PreviousTradeCount, LifetimeHighDate, TradingStatusDetails, ClosingAsk, Low, Volume, PreviousTradingDate, PreviousCumulativeValue, TradeCount, Close, TradingStatusReason, LimitHighLowTime, AskSize, CloseCumulativeVolumeDate, TradingStatus, UpdateId, LocalCode, ClosingQuoteDate, BidSize, Open, QuoteLotSize, PreviousCumulativeVolumeDate, Ask, TradeDate, LowTime, CloseStatus, OpenInterestDate, PreviousCumulativeVolume, Context, TradeExchange, LowCondition, TradeTime, ClosingAskExchange, Week52Low, BidExchange, LifetimeLow, LifetimeLowDate, CloseCumulativeValue, PrePostMarketTrade, PreviousOpenInterestDate, ClientIdentity, ExpirationDate, ResetDate, LowExchange, AskTime, BidTime, PrePostMarketTradeSize, LastUpdateDate, AskExchange, PreviousTradeTime, CreateDate, CloseCumulativeVolumeStatus, LimitLowPrice, Last, HighExchange, PreviousAsk, LotSize, PreviousTradeLow, PercentChange, PreviousTradeHigh, PreviousCloseDate, Week52High, TradingStatusReasonDetails, CloseCumulativeValueStatus, OpenInterest, EntityType, State, ClosingBid, ClosingBidExchange, PreviousPercentChange, CloseCumulativeVolume, Symbol, HighTime, CloseExchange, CumulativeValue, PreviousOpenInterest, HighCondition, PreviousQuoteDate, ExpirationType, ShortSalePriceRestrictedDescription, Bid, OpenCondition, LifetimeHigh, OptionType, High, StrikePrice, Change, TradeCondition, LimitHighPrice, PermissionId]</t>
   </si>
   <si>
@@ -189,27 +180,9 @@
     <t>Topic_Response_ObjectName</t>
   </si>
   <si>
-    <t>Verify_Opt_Subscribe_Bulk_MarketData_TC0002</t>
-  </si>
-  <si>
-    <t>Verify_Opt_Subscribe_Bulk_MarketData_TC0003</t>
-  </si>
-  <si>
-    <t>Verify_Opt_Subscribe_Bulk_MarketData_TC0004</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
-    <t>Verify_Opt_Subscribe_MarketData_TC0002</t>
-  </si>
-  <si>
-    <t>Verify_Opt_Subscribe_MarketData_TC0003</t>
-  </si>
-  <si>
-    <t>Verify_Opt_Subscribe_MarketData_TC0004</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -237,41 +210,182 @@
     <t>Verify_Opt_UnSubscribe_Bulk_MarketData_TC0004</t>
   </si>
   <si>
-    <t>Verify_Opt_Topic_TC0002</t>
-  </si>
-  <si>
-    <t>Verify_Opt_Topic_TC0003</t>
-  </si>
-  <si>
-    <t>Verify_Opt_Topic_TC0004</t>
-  </si>
-  <si>
-    <t>Verify_Opt_Topic_TC0005</t>
-  </si>
-  <si>
     <t>AA</t>
   </si>
   <si>
     <t>Subscribe_Bulk_NoSnapshot_TestCases</t>
   </si>
   <si>
-    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TC0001</t>
-  </si>
-  <si>
-    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TC0002</t>
-  </si>
-  <si>
-    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TC0003</t>
-  </si>
-  <si>
-    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TC0004</t>
+    <t>Success!</t>
+  </si>
+  <si>
+    <t>AA123</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Topic_TestCase_VTRAD-C475-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Topic_TestCase_VTRAD-C475-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Topic_TestCase_VTRAD-C475-C</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Topic_TestCase_VTRAD-C476-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Topic_TestCase_VTRAD-C476-A</t>
+  </si>
+  <si>
+    <t>MSFT332</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_MarketData_TestCase_VTRAD-C471-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_MarketData_TestCase_VTRAD-C471-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_Bulk_MarketData_TestCase_VTRAD-C453-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_Bulk_MarketData_TestCase_VTRAD-C453-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_Bulk_MarketData_TestCase_VTRAD-C454-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_Bulk_MarketData_TestCase_VTRAD-C454-B</t>
+  </si>
+  <si>
+    <t>QQQ123</t>
+  </si>
+  <si>
+    <t>MSFT123</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C468-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C468-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C468-C</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C469-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C468-D</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C469-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C469-C</t>
+  </si>
+  <si>
+    <t>IBM258</t>
+  </si>
+  <si>
+    <t>A365</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C470</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TestCase_VTRAD-C448-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TestCase_VTRAD-C448-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TestCase_VTRAD-C449-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TestCase_VTRAD-C448-C</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TestCase_VTRAD-C448-D</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TestCase_VTRAD-C449-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_NoSnapshot_MarketData_TestCase_VTRAD-C449-C</t>
+  </si>
+  <si>
+    <t>IBM123</t>
+  </si>
+  <si>
+    <t>A258</t>
+  </si>
+  <si>
+    <t>QQQ321</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_MarketData_TestCase_VTRAD-C472-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_MarketData_TestCase_VTRAD-C471-C</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_MarketData_TestCase_VTRAD-C471-D</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_MarketData_TestCase_VTRAD-C472-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_UnSubscribe_MarketData_TestCase_VTRAD-C472-C</t>
+  </si>
+  <si>
+    <t>A123</t>
+  </si>
+  <si>
+    <t>QQQ365</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_MarketData_TestCase_VTRAD-C473-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_MarketData_TestCase_VTRAD-C473-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_MarketData_TestCase_VTRAD-C473-C</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_MarketData_TestCase_VTRAD-C474-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_MarketData_TestCase_VTRAD-C474-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_MarketData_TestCase_VTRAD-C473-D</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_Bulk_MarketData_TestCase_VTRAD-C474-C</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C452-A</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C452-B</t>
+  </si>
+  <si>
+    <t>Verify_Opt_Subscribe_MarketData_TestCase_VTRAD-C452-C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +417,17 @@
     <font>
       <sz val="9"/>
       <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -342,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -350,12 +475,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,12 +770,13 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
@@ -656,7 +788,7 @@
         <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -673,10 +805,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -693,10 +825,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -705,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
@@ -713,10 +845,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -724,8 +856,8 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>59</v>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
@@ -733,10 +865,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -745,7 +877,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
@@ -753,10 +885,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -765,7 +897,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
@@ -782,7 +914,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C78390D-BD0C-4F58-80E1-D4EAF5F6FC8D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -796,10 +930,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>15</v>
@@ -819,10 +953,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -842,10 +976,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -865,10 +999,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -888,10 +1022,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -918,182 +1052,406 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F364E6-3960-41EC-8208-7CD92A199C3C}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="5" customWidth="1"/>
-    <col min="3" max="6" width="47.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="63.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="9" customWidth="1"/>
+    <col min="3" max="6" width="47.140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="255.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="J1" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="9">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="I2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="9">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="9">
+        <v>3</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="9">
+        <v>4</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="9">
+        <v>4</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="9">
+        <v>4</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="H10" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="1">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="H11" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="1">
-        <v>4</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>43</v>
+      <c r="H12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1105,229 +1463,353 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0191CE-EB5C-4C7A-A2C4-22940355F57C}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="6" width="47.140625" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="167" customWidth="1"/>
-    <col min="11" max="11" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="8" customWidth="1"/>
+    <col min="3" max="6" width="47.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="167" style="8" customWidth="1"/>
+    <col min="11" max="11" width="47.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="J1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="8">
         <v>1</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="I2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="L2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="8">
         <v>2</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="I3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="4" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="L3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="8">
         <v>3</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="I4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="4" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="L4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="4" t="s">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="4">
-        <v>4</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="H5" s="8">
+        <v>4</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>18</v>
+      <c r="L5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="8">
+        <v>3</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="8">
+        <v>2</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="8">
+        <v>3</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1338,15 +1820,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E83D13-0522-442A-A3AF-A865C1C21765}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="45.140625" customWidth="1"/>
@@ -1358,10 +1840,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1379,24 +1861,24 @@
         <v>12</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1414,7 +1896,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -1423,15 +1905,15 @@
         <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1440,7 +1922,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
@@ -1449,24 +1931,24 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1474,8 +1956,8 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>59</v>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
@@ -1484,7 +1966,7 @@
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -1493,15 +1975,15 @@
         <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1510,7 +1992,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
@@ -1519,16 +2001,121 @@
         <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6">
+        <v>-1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7">
+        <v>-2</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8">
+        <v>-8</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1542,13 +2129,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A97062F-F8F8-4DA2-BE61-017920E2ED20}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="45.140625" customWidth="1"/>
@@ -1563,10 +2150,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1584,16 +2171,16 @@
         <v>12</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>24</v>
@@ -1607,10 +2194,10 @@
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1628,7 +2215,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -1637,7 +2224,7 @@
         <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
@@ -1646,15 +2233,15 @@
         <v>6</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1663,7 +2250,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
@@ -1672,16 +2259,16 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L3" t="s">
         <v>22</v>
@@ -1690,15 +2277,15 @@
         <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1706,8 +2293,8 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>59</v>
+      <c r="E4" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
@@ -1716,7 +2303,7 @@
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -1725,7 +2312,7 @@
         <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L4" t="s">
         <v>22</v>
@@ -1734,15 +2321,15 @@
         <v>6</v>
       </c>
       <c r="N4" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1751,7 +2338,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
@@ -1760,16 +2347,16 @@
         <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L5" t="s">
         <v>22</v>
@@ -1778,7 +2365,7 @@
         <v>6</v>
       </c>
       <c r="N5" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1790,15 +2377,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D99B42-91CA-4CCD-8869-CE1A23CE9A41}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="45.140625" customWidth="1"/>
@@ -1813,10 +2400,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1834,16 +2421,16 @@
         <v>12</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>24</v>
@@ -1857,10 +2444,10 @@
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1868,7 +2455,7 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1878,7 +2465,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -1887,7 +2474,7 @@
         <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L2" t="s">
         <v>25</v>
@@ -1901,10 +2488,10 @@
     </row>
     <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1912,8 +2499,8 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>58</v>
+      <c r="E3" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
@@ -1922,16 +2509,16 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L3" t="s">
         <v>25</v>
@@ -1945,10 +2532,10 @@
     </row>
     <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1956,8 +2543,8 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>59</v>
+      <c r="E4" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
@@ -1966,7 +2553,7 @@
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -1975,7 +2562,7 @@
         <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L4" t="s">
         <v>25</v>
@@ -1989,10 +2576,10 @@
     </row>
     <row r="5" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -2000,8 +2587,8 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>60</v>
+      <c r="E5" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
@@ -2010,16 +2597,16 @@
         <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L5" t="s">
         <v>25</v>
@@ -2028,6 +2615,226 @@
         <v>6</v>
       </c>
       <c r="N5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6">
+        <v>-5</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7">
+        <v>-2</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2043,7 +2850,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,10 +2866,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>20</v>
@@ -2082,10 +2889,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -2100,15 +2907,15 @@
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -2117,21 +2924,21 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -2139,22 +2946,22 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>59</v>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -2163,13 +2970,13 @@
         <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2201,10 +3008,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>24</v>
@@ -2213,10 +3020,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>17</v>
@@ -2227,10 +3034,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -2239,7 +3046,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -2253,10 +3060,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -2265,10 +3072,10 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
@@ -2279,10 +3086,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -2291,7 +3098,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -2305,10 +3112,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -2317,10 +3124,10 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>6</v>
@@ -2356,10 +3163,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>24</v>
@@ -2376,10 +3183,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>

</xml_diff>